<commit_message>
capturing miniscule progress on spreadsheet
</commit_message>
<xml_diff>
--- a/c++/PETSc_Tests/NonLinear-Verification.xlsx
+++ b/c++/PETSc_Tests/NonLinear-Verification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonyalberti/Documents/projects/Fctn_Src/c++/PETSc_Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78705516-9BEF-0440-AC54-5764E727EF18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E93C48B-7AB8-3547-AA1E-3F3B0BED9E32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2180" yWindow="460" windowWidth="26620" windowHeight="17540" xr2:uid="{A64FA9E8-8B1C-4A42-B432-8621287DF68E}"/>
   </bookViews>
@@ -8975,8 +8975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9C1D7F-C241-6C4B-A1E9-89DBFAC3176A}">
   <dimension ref="A1:AI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>